<commit_message>
5/28 finished 2nd work
</commit_message>
<xml_diff>
--- a/syspro_2nd/d_signal/d_wave_inv_dft.xlsx
+++ b/syspro_2nd/d_signal/d_wave_inv_dft.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chasolaptop/test/univ/cfile_syspro/syspro_2nd/d_signal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chasolaptop/test/univ/cfile_syspro/syspro_2nd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2000F1FC-9C4A-2B47-B2B4-B4D88AD3983A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6E8156-0780-8D44-B123-A9C7CB9B107F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="960" windowWidth="27900" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="28300" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="d_wave_inv_dft" sheetId="1" r:id="rId1"/>
@@ -2295,604 +2295,604 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="186">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="193">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="196">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="197">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="200">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="201">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="202">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="203">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="204">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="205">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="206">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="207">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="208">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="209">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="210">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="211">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="212">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="213">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="214">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="215">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="216">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="217">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="218">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="219">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="220">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="221">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="222">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="223">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="224">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="225">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="226">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="227">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="228">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="229">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="230">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="231">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="232">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="233">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="234">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="235">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="236">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="237">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="238">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="239">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="240">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="241">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="242">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="243">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="244">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="245">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="246">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="247">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="248">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="249">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="250">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="251">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="252">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="253">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="254">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="255">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="256">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="257">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="258">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="259">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="260">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="261">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="262">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="263">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="264">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="265">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="266">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="267">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="268">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="269">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="270">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="271">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="272">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="273">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="274">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="275">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="276">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="277">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="278">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="279">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="280">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="281">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="282">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="283">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="284">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="285">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="286">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="287">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="288">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="289">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="290">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="291">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="292">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="293">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="294">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="295">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="296">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="297">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="298">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="299">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="300">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="301">
                   <c:v>-1</c:v>
@@ -3197,7 +3197,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FDF5-1D4D-9890-52C1B066DD01}"/>
+              <c16:uniqueId val="{00000000-F657-D94E-AA99-ED1C4E4CA693}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3209,11 +3209,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1174453504"/>
-        <c:axId val="1174442640"/>
+        <c:axId val="1683058864"/>
+        <c:axId val="1729393872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1174453504"/>
+        <c:axId val="1683058864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3270,12 +3270,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1174442640"/>
+        <c:crossAx val="1729393872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1174442640"/>
+        <c:axId val="1729393872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3332,7 +3332,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1174453504"/>
+        <c:crossAx val="1683058864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4954,604 +4954,604 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="186">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="189">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="191">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="192">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="193">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="196">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="197">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="200">
-                  <c:v>-1</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="201">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="202">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="203">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="204">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="205">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="206">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="207">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="208">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="209">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="210">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="211">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="212">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="213">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="214">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="215">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="216">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="217">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="218">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="219">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="220">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="221">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="222">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="223">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="224">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="225">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="226">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="227">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="228">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="229">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="230">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="231">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="232">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="233">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="234">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="235">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="236">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="237">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="238">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="239">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="240">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="241">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="242">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="243">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="244">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="245">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="246">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="247">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="248">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="249">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="250">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="251">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="252">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="253">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="254">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="255">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="256">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="257">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="258">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="259">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="260">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="261">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="262">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="263">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="264">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="265">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="266">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="267">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="268">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="269">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="270">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="271">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="272">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="273">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="274">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="275">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="276">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="277">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="278">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="279">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="280">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="281">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="282">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="283">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="284">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="285">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="286">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="287">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="288">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="289">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="290">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="291">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="292">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="293">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="294">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="295">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="296">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="297">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="298">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="299">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="300">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="301">
                   <c:v>-1</c:v>
@@ -5856,7 +5856,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7A82-E146-855C-0F89D729C444}"/>
+              <c16:uniqueId val="{00000000-DE72-8045-96E7-058D6B01218D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5868,11 +5868,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1174453504"/>
-        <c:axId val="1174442640"/>
+        <c:axId val="1683058864"/>
+        <c:axId val="1729393872"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1174453504"/>
+        <c:axId val="1683058864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5929,12 +5929,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1174442640"/>
+        <c:crossAx val="1729393872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1174442640"/>
+        <c:axId val="1729393872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5991,7 +5991,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1174453504"/>
+        <c:crossAx val="1683058864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7163,23 +7163,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>660400</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>203200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="グラフ 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27037D1C-4250-CD4F-BACA-C812805AD024}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9639CA7-62DF-9642-A290-2C22F90C450F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7201,13 +7201,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>762000</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>203200</xdr:rowOff>
@@ -7217,7 +7217,7 @@
         <xdr:cNvPr id="4" name="グラフ 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56853C48-1B76-494E-9B4A-F9370C48AE8A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8ECE33E-389F-0B43-BC90-FBEC2CB60968}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7540,7 +7540,7 @@
   <dimension ref="A1:B400"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -8358,7 +8358,7 @@
         <v>101</v>
       </c>
       <c r="B102">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -8366,7 +8366,7 @@
         <v>102</v>
       </c>
       <c r="B103">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -8374,7 +8374,7 @@
         <v>103</v>
       </c>
       <c r="B104">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -8382,7 +8382,7 @@
         <v>104</v>
       </c>
       <c r="B105">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -8390,7 +8390,7 @@
         <v>105</v>
       </c>
       <c r="B106">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -8398,7 +8398,7 @@
         <v>106</v>
       </c>
       <c r="B107">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -8406,7 +8406,7 @@
         <v>107</v>
       </c>
       <c r="B108">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -8414,7 +8414,7 @@
         <v>108</v>
       </c>
       <c r="B109">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -8422,7 +8422,7 @@
         <v>109</v>
       </c>
       <c r="B110">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -8430,7 +8430,7 @@
         <v>110</v>
       </c>
       <c r="B111">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -8438,7 +8438,7 @@
         <v>111</v>
       </c>
       <c r="B112">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -8446,7 +8446,7 @@
         <v>112</v>
       </c>
       <c r="B113">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -8454,7 +8454,7 @@
         <v>113</v>
       </c>
       <c r="B114">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -8462,7 +8462,7 @@
         <v>114</v>
       </c>
       <c r="B115">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -8470,7 +8470,7 @@
         <v>115</v>
       </c>
       <c r="B116">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -8478,7 +8478,7 @@
         <v>116</v>
       </c>
       <c r="B117">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -8486,7 +8486,7 @@
         <v>117</v>
       </c>
       <c r="B118">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -8494,7 +8494,7 @@
         <v>118</v>
       </c>
       <c r="B119">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -8502,7 +8502,7 @@
         <v>119</v>
       </c>
       <c r="B120">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -8510,7 +8510,7 @@
         <v>120</v>
       </c>
       <c r="B121">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -8518,7 +8518,7 @@
         <v>121</v>
       </c>
       <c r="B122">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -8526,7 +8526,7 @@
         <v>122</v>
       </c>
       <c r="B123">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -8534,7 +8534,7 @@
         <v>123</v>
       </c>
       <c r="B124">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -8542,7 +8542,7 @@
         <v>124</v>
       </c>
       <c r="B125">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -8550,7 +8550,7 @@
         <v>125</v>
       </c>
       <c r="B126">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -8558,7 +8558,7 @@
         <v>126</v>
       </c>
       <c r="B127">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -8566,7 +8566,7 @@
         <v>127</v>
       </c>
       <c r="B128">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -8574,7 +8574,7 @@
         <v>128</v>
       </c>
       <c r="B129">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -8582,7 +8582,7 @@
         <v>129</v>
       </c>
       <c r="B130">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -8590,7 +8590,7 @@
         <v>130</v>
       </c>
       <c r="B131">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -8598,7 +8598,7 @@
         <v>131</v>
       </c>
       <c r="B132">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -8606,7 +8606,7 @@
         <v>132</v>
       </c>
       <c r="B133">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -8614,7 +8614,7 @@
         <v>133</v>
       </c>
       <c r="B134">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -8622,7 +8622,7 @@
         <v>134</v>
       </c>
       <c r="B135">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -8630,7 +8630,7 @@
         <v>135</v>
       </c>
       <c r="B136">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -8638,7 +8638,7 @@
         <v>136</v>
       </c>
       <c r="B137">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -8646,7 +8646,7 @@
         <v>137</v>
       </c>
       <c r="B138">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -8654,7 +8654,7 @@
         <v>138</v>
       </c>
       <c r="B139">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -8662,7 +8662,7 @@
         <v>139</v>
       </c>
       <c r="B140">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -8670,7 +8670,7 @@
         <v>140</v>
       </c>
       <c r="B141">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -8678,7 +8678,7 @@
         <v>141</v>
       </c>
       <c r="B142">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -8686,7 +8686,7 @@
         <v>142</v>
       </c>
       <c r="B143">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -8694,7 +8694,7 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -8702,7 +8702,7 @@
         <v>144</v>
       </c>
       <c r="B145">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -8710,7 +8710,7 @@
         <v>145</v>
       </c>
       <c r="B146">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -8718,7 +8718,7 @@
         <v>146</v>
       </c>
       <c r="B147">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -8726,7 +8726,7 @@
         <v>147</v>
       </c>
       <c r="B148">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -8734,7 +8734,7 @@
         <v>148</v>
       </c>
       <c r="B149">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -8742,7 +8742,7 @@
         <v>149</v>
       </c>
       <c r="B150">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -8750,7 +8750,7 @@
         <v>150</v>
       </c>
       <c r="B151">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -8758,7 +8758,7 @@
         <v>151</v>
       </c>
       <c r="B152">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -8766,7 +8766,7 @@
         <v>152</v>
       </c>
       <c r="B153">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -8774,7 +8774,7 @@
         <v>153</v>
       </c>
       <c r="B154">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -8782,7 +8782,7 @@
         <v>154</v>
       </c>
       <c r="B155">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -8790,7 +8790,7 @@
         <v>155</v>
       </c>
       <c r="B156">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -8798,7 +8798,7 @@
         <v>156</v>
       </c>
       <c r="B157">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -8806,7 +8806,7 @@
         <v>157</v>
       </c>
       <c r="B158">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -8814,7 +8814,7 @@
         <v>158</v>
       </c>
       <c r="B159">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -8822,7 +8822,7 @@
         <v>159</v>
       </c>
       <c r="B160">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -8830,7 +8830,7 @@
         <v>160</v>
       </c>
       <c r="B161">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -8838,7 +8838,7 @@
         <v>161</v>
       </c>
       <c r="B162">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -8846,7 +8846,7 @@
         <v>162</v>
       </c>
       <c r="B163">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -8854,7 +8854,7 @@
         <v>163</v>
       </c>
       <c r="B164">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165" spans="1:2">
@@ -8862,7 +8862,7 @@
         <v>164</v>
       </c>
       <c r="B165">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="166" spans="1:2">
@@ -8870,7 +8870,7 @@
         <v>165</v>
       </c>
       <c r="B166">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="167" spans="1:2">
@@ -8878,7 +8878,7 @@
         <v>166</v>
       </c>
       <c r="B167">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168" spans="1:2">
@@ -8886,7 +8886,7 @@
         <v>167</v>
       </c>
       <c r="B168">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169" spans="1:2">
@@ -8894,7 +8894,7 @@
         <v>168</v>
       </c>
       <c r="B169">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170" spans="1:2">
@@ -8902,7 +8902,7 @@
         <v>169</v>
       </c>
       <c r="B170">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -8910,7 +8910,7 @@
         <v>170</v>
       </c>
       <c r="B171">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172" spans="1:2">
@@ -8918,7 +8918,7 @@
         <v>171</v>
       </c>
       <c r="B172">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173" spans="1:2">
@@ -8926,7 +8926,7 @@
         <v>172</v>
       </c>
       <c r="B173">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="174" spans="1:2">
@@ -8934,7 +8934,7 @@
         <v>173</v>
       </c>
       <c r="B174">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175" spans="1:2">
@@ -8942,7 +8942,7 @@
         <v>174</v>
       </c>
       <c r="B175">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176" spans="1:2">
@@ -8950,7 +8950,7 @@
         <v>175</v>
       </c>
       <c r="B176">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177" spans="1:2">
@@ -8958,7 +8958,7 @@
         <v>176</v>
       </c>
       <c r="B177">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="178" spans="1:2">
@@ -8966,7 +8966,7 @@
         <v>177</v>
       </c>
       <c r="B178">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="179" spans="1:2">
@@ -8974,7 +8974,7 @@
         <v>178</v>
       </c>
       <c r="B179">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180" spans="1:2">
@@ -8982,7 +8982,7 @@
         <v>179</v>
       </c>
       <c r="B180">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="181" spans="1:2">
@@ -8990,7 +8990,7 @@
         <v>180</v>
       </c>
       <c r="B181">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -8998,7 +8998,7 @@
         <v>181</v>
       </c>
       <c r="B182">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="183" spans="1:2">
@@ -9006,7 +9006,7 @@
         <v>182</v>
       </c>
       <c r="B183">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -9014,7 +9014,7 @@
         <v>183</v>
       </c>
       <c r="B184">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="185" spans="1:2">
@@ -9022,7 +9022,7 @@
         <v>184</v>
       </c>
       <c r="B185">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="186" spans="1:2">
@@ -9030,7 +9030,7 @@
         <v>185</v>
       </c>
       <c r="B186">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187" spans="1:2">
@@ -9038,7 +9038,7 @@
         <v>186</v>
       </c>
       <c r="B187">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="188" spans="1:2">
@@ -9046,7 +9046,7 @@
         <v>187</v>
       </c>
       <c r="B188">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="189" spans="1:2">
@@ -9054,7 +9054,7 @@
         <v>188</v>
       </c>
       <c r="B189">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190" spans="1:2">
@@ -9062,7 +9062,7 @@
         <v>189</v>
       </c>
       <c r="B190">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="191" spans="1:2">
@@ -9070,7 +9070,7 @@
         <v>190</v>
       </c>
       <c r="B191">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="192" spans="1:2">
@@ -9078,7 +9078,7 @@
         <v>191</v>
       </c>
       <c r="B192">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="193" spans="1:2">
@@ -9086,7 +9086,7 @@
         <v>192</v>
       </c>
       <c r="B193">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194" spans="1:2">
@@ -9094,7 +9094,7 @@
         <v>193</v>
       </c>
       <c r="B194">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195" spans="1:2">
@@ -9102,7 +9102,7 @@
         <v>194</v>
       </c>
       <c r="B195">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -9110,7 +9110,7 @@
         <v>195</v>
       </c>
       <c r="B196">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="197" spans="1:2">
@@ -9118,7 +9118,7 @@
         <v>196</v>
       </c>
       <c r="B197">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -9126,7 +9126,7 @@
         <v>197</v>
       </c>
       <c r="B198">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -9134,7 +9134,7 @@
         <v>198</v>
       </c>
       <c r="B199">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="200" spans="1:2">
@@ -9142,7 +9142,7 @@
         <v>199</v>
       </c>
       <c r="B200">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="201" spans="1:2">
@@ -9150,7 +9150,7 @@
         <v>200</v>
       </c>
       <c r="B201">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="202" spans="1:2">
@@ -9158,7 +9158,7 @@
         <v>201</v>
       </c>
       <c r="B202">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -9166,7 +9166,7 @@
         <v>202</v>
       </c>
       <c r="B203">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="204" spans="1:2">
@@ -9174,7 +9174,7 @@
         <v>203</v>
       </c>
       <c r="B204">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="205" spans="1:2">
@@ -9182,7 +9182,7 @@
         <v>204</v>
       </c>
       <c r="B205">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="206" spans="1:2">
@@ -9190,7 +9190,7 @@
         <v>205</v>
       </c>
       <c r="B206">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="207" spans="1:2">
@@ -9198,7 +9198,7 @@
         <v>206</v>
       </c>
       <c r="B207">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="208" spans="1:2">
@@ -9206,7 +9206,7 @@
         <v>207</v>
       </c>
       <c r="B208">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="209" spans="1:2">
@@ -9214,7 +9214,7 @@
         <v>208</v>
       </c>
       <c r="B209">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="210" spans="1:2">
@@ -9222,7 +9222,7 @@
         <v>209</v>
       </c>
       <c r="B210">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -9230,7 +9230,7 @@
         <v>210</v>
       </c>
       <c r="B211">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -9238,7 +9238,7 @@
         <v>211</v>
       </c>
       <c r="B212">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="213" spans="1:2">
@@ -9246,7 +9246,7 @@
         <v>212</v>
       </c>
       <c r="B213">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="214" spans="1:2">
@@ -9254,7 +9254,7 @@
         <v>213</v>
       </c>
       <c r="B214">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="215" spans="1:2">
@@ -9262,7 +9262,7 @@
         <v>214</v>
       </c>
       <c r="B215">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="216" spans="1:2">
@@ -9270,7 +9270,7 @@
         <v>215</v>
       </c>
       <c r="B216">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="217" spans="1:2">
@@ -9278,7 +9278,7 @@
         <v>216</v>
       </c>
       <c r="B217">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="218" spans="1:2">
@@ -9286,7 +9286,7 @@
         <v>217</v>
       </c>
       <c r="B218">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="219" spans="1:2">
@@ -9294,7 +9294,7 @@
         <v>218</v>
       </c>
       <c r="B219">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="220" spans="1:2">
@@ -9302,7 +9302,7 @@
         <v>219</v>
       </c>
       <c r="B220">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="221" spans="1:2">
@@ -9310,7 +9310,7 @@
         <v>220</v>
       </c>
       <c r="B221">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="222" spans="1:2">
@@ -9318,7 +9318,7 @@
         <v>221</v>
       </c>
       <c r="B222">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="223" spans="1:2">
@@ -9326,7 +9326,7 @@
         <v>222</v>
       </c>
       <c r="B223">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="224" spans="1:2">
@@ -9334,7 +9334,7 @@
         <v>223</v>
       </c>
       <c r="B224">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="225" spans="1:2">
@@ -9342,7 +9342,7 @@
         <v>224</v>
       </c>
       <c r="B225">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="226" spans="1:2">
@@ -9350,7 +9350,7 @@
         <v>225</v>
       </c>
       <c r="B226">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="227" spans="1:2">
@@ -9358,7 +9358,7 @@
         <v>226</v>
       </c>
       <c r="B227">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="228" spans="1:2">
@@ -9366,7 +9366,7 @@
         <v>227</v>
       </c>
       <c r="B228">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="229" spans="1:2">
@@ -9374,7 +9374,7 @@
         <v>228</v>
       </c>
       <c r="B229">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="230" spans="1:2">
@@ -9382,7 +9382,7 @@
         <v>229</v>
       </c>
       <c r="B230">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="231" spans="1:2">
@@ -9390,7 +9390,7 @@
         <v>230</v>
       </c>
       <c r="B231">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="232" spans="1:2">
@@ -9398,7 +9398,7 @@
         <v>231</v>
       </c>
       <c r="B232">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="233" spans="1:2">
@@ -9406,7 +9406,7 @@
         <v>232</v>
       </c>
       <c r="B233">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="234" spans="1:2">
@@ -9414,7 +9414,7 @@
         <v>233</v>
       </c>
       <c r="B234">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="235" spans="1:2">
@@ -9422,7 +9422,7 @@
         <v>234</v>
       </c>
       <c r="B235">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="236" spans="1:2">
@@ -9430,7 +9430,7 @@
         <v>235</v>
       </c>
       <c r="B236">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="237" spans="1:2">
@@ -9438,7 +9438,7 @@
         <v>236</v>
       </c>
       <c r="B237">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="238" spans="1:2">
@@ -9446,7 +9446,7 @@
         <v>237</v>
       </c>
       <c r="B238">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="239" spans="1:2">
@@ -9454,7 +9454,7 @@
         <v>238</v>
       </c>
       <c r="B239">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="240" spans="1:2">
@@ -9462,7 +9462,7 @@
         <v>239</v>
       </c>
       <c r="B240">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="241" spans="1:2">
@@ -9470,7 +9470,7 @@
         <v>240</v>
       </c>
       <c r="B241">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="242" spans="1:2">
@@ -9478,7 +9478,7 @@
         <v>241</v>
       </c>
       <c r="B242">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="243" spans="1:2">
@@ -9486,7 +9486,7 @@
         <v>242</v>
       </c>
       <c r="B243">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="244" spans="1:2">
@@ -9494,7 +9494,7 @@
         <v>243</v>
       </c>
       <c r="B244">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="245" spans="1:2">
@@ -9502,7 +9502,7 @@
         <v>244</v>
       </c>
       <c r="B245">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="246" spans="1:2">
@@ -9510,7 +9510,7 @@
         <v>245</v>
       </c>
       <c r="B246">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="247" spans="1:2">
@@ -9518,7 +9518,7 @@
         <v>246</v>
       </c>
       <c r="B247">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="248" spans="1:2">
@@ -9526,7 +9526,7 @@
         <v>247</v>
       </c>
       <c r="B248">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="249" spans="1:2">
@@ -9534,7 +9534,7 @@
         <v>248</v>
       </c>
       <c r="B249">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="250" spans="1:2">
@@ -9542,7 +9542,7 @@
         <v>249</v>
       </c>
       <c r="B250">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="251" spans="1:2">
@@ -9550,7 +9550,7 @@
         <v>250</v>
       </c>
       <c r="B251">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="252" spans="1:2">
@@ -9558,7 +9558,7 @@
         <v>251</v>
       </c>
       <c r="B252">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="253" spans="1:2">
@@ -9566,7 +9566,7 @@
         <v>252</v>
       </c>
       <c r="B253">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="254" spans="1:2">
@@ -9574,7 +9574,7 @@
         <v>253</v>
       </c>
       <c r="B254">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="255" spans="1:2">
@@ -9582,7 +9582,7 @@
         <v>254</v>
       </c>
       <c r="B255">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="256" spans="1:2">
@@ -9590,7 +9590,7 @@
         <v>255</v>
       </c>
       <c r="B256">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="257" spans="1:2">
@@ -9598,7 +9598,7 @@
         <v>256</v>
       </c>
       <c r="B257">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="258" spans="1:2">
@@ -9606,7 +9606,7 @@
         <v>257</v>
       </c>
       <c r="B258">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="259" spans="1:2">
@@ -9614,7 +9614,7 @@
         <v>258</v>
       </c>
       <c r="B259">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="260" spans="1:2">
@@ -9622,7 +9622,7 @@
         <v>259</v>
       </c>
       <c r="B260">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="261" spans="1:2">
@@ -9630,7 +9630,7 @@
         <v>260</v>
       </c>
       <c r="B261">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="262" spans="1:2">
@@ -9638,7 +9638,7 @@
         <v>261</v>
       </c>
       <c r="B262">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="263" spans="1:2">
@@ -9646,7 +9646,7 @@
         <v>262</v>
       </c>
       <c r="B263">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="264" spans="1:2">
@@ -9654,7 +9654,7 @@
         <v>263</v>
       </c>
       <c r="B264">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="265" spans="1:2">
@@ -9662,7 +9662,7 @@
         <v>264</v>
       </c>
       <c r="B265">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="266" spans="1:2">
@@ -9670,7 +9670,7 @@
         <v>265</v>
       </c>
       <c r="B266">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="267" spans="1:2">
@@ -9678,7 +9678,7 @@
         <v>266</v>
       </c>
       <c r="B267">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="268" spans="1:2">
@@ -9686,7 +9686,7 @@
         <v>267</v>
       </c>
       <c r="B268">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="269" spans="1:2">
@@ -9694,7 +9694,7 @@
         <v>268</v>
       </c>
       <c r="B269">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="270" spans="1:2">
@@ -9702,7 +9702,7 @@
         <v>269</v>
       </c>
       <c r="B270">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="271" spans="1:2">
@@ -9710,7 +9710,7 @@
         <v>270</v>
       </c>
       <c r="B271">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="272" spans="1:2">
@@ -9718,7 +9718,7 @@
         <v>271</v>
       </c>
       <c r="B272">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="273" spans="1:2">
@@ -9726,7 +9726,7 @@
         <v>272</v>
       </c>
       <c r="B273">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="274" spans="1:2">
@@ -9734,7 +9734,7 @@
         <v>273</v>
       </c>
       <c r="B274">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="275" spans="1:2">
@@ -9742,7 +9742,7 @@
         <v>274</v>
       </c>
       <c r="B275">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="276" spans="1:2">
@@ -9750,7 +9750,7 @@
         <v>275</v>
       </c>
       <c r="B276">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="277" spans="1:2">
@@ -9758,7 +9758,7 @@
         <v>276</v>
       </c>
       <c r="B277">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="278" spans="1:2">
@@ -9766,7 +9766,7 @@
         <v>277</v>
       </c>
       <c r="B278">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="279" spans="1:2">
@@ -9774,7 +9774,7 @@
         <v>278</v>
       </c>
       <c r="B279">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="280" spans="1:2">
@@ -9782,7 +9782,7 @@
         <v>279</v>
       </c>
       <c r="B280">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="281" spans="1:2">
@@ -9790,7 +9790,7 @@
         <v>280</v>
       </c>
       <c r="B281">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="282" spans="1:2">
@@ -9798,7 +9798,7 @@
         <v>281</v>
       </c>
       <c r="B282">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="283" spans="1:2">
@@ -9806,7 +9806,7 @@
         <v>282</v>
       </c>
       <c r="B283">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="284" spans="1:2">
@@ -9814,7 +9814,7 @@
         <v>283</v>
       </c>
       <c r="B284">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="285" spans="1:2">
@@ -9822,7 +9822,7 @@
         <v>284</v>
       </c>
       <c r="B285">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="286" spans="1:2">
@@ -9830,7 +9830,7 @@
         <v>285</v>
       </c>
       <c r="B286">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="287" spans="1:2">
@@ -9838,7 +9838,7 @@
         <v>286</v>
       </c>
       <c r="B287">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="288" spans="1:2">
@@ -9846,7 +9846,7 @@
         <v>287</v>
       </c>
       <c r="B288">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="289" spans="1:2">
@@ -9854,7 +9854,7 @@
         <v>288</v>
       </c>
       <c r="B289">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="290" spans="1:2">
@@ -9862,7 +9862,7 @@
         <v>289</v>
       </c>
       <c r="B290">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="291" spans="1:2">
@@ -9870,7 +9870,7 @@
         <v>290</v>
       </c>
       <c r="B291">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="292" spans="1:2">
@@ -9878,7 +9878,7 @@
         <v>291</v>
       </c>
       <c r="B292">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="293" spans="1:2">
@@ -9886,7 +9886,7 @@
         <v>292</v>
       </c>
       <c r="B293">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="294" spans="1:2">
@@ -9894,7 +9894,7 @@
         <v>293</v>
       </c>
       <c r="B294">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="295" spans="1:2">
@@ -9902,7 +9902,7 @@
         <v>294</v>
       </c>
       <c r="B295">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="296" spans="1:2">
@@ -9910,7 +9910,7 @@
         <v>295</v>
       </c>
       <c r="B296">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="297" spans="1:2">
@@ -9918,7 +9918,7 @@
         <v>296</v>
       </c>
       <c r="B297">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="298" spans="1:2">
@@ -9926,7 +9926,7 @@
         <v>297</v>
       </c>
       <c r="B298">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="299" spans="1:2">
@@ -9934,7 +9934,7 @@
         <v>298</v>
       </c>
       <c r="B299">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="300" spans="1:2">
@@ -9942,7 +9942,7 @@
         <v>299</v>
       </c>
       <c r="B300">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="301" spans="1:2">
@@ -9950,7 +9950,7 @@
         <v>300</v>
       </c>
       <c r="B301">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="302" spans="1:2">

</xml_diff>